<commit_message>
Batch validation, add batch delete batch commit
</commit_message>
<xml_diff>
--- a/Team11-UITesters/src/test/resources/InputData/TestData.xlsx
+++ b/Team11-UITesters/src/test/resources/InputData/TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrav\eclipse-workspace\Team11-UITesters\src\test\resources\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirti\git\Team11-UITesters\Team11-UITesters\src\test\resources\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345B5862-A2A0-41CB-B416-CD2C15BAB9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBDF7D3-5C96-48D7-A870-719A72F4480B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="3" r:id="rId1"/>
+    <sheet name="Login" sheetId="8" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="4" r:id="rId2"/>
     <sheet name="Program" sheetId="5" r:id="rId3"/>
     <sheet name="Batch" sheetId="6" r:id="rId4"/>
@@ -24,120 +24,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
-  <si>
-    <t>UserName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Confirmpwd</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>errorMessage</t>
-  </si>
-  <si>
-    <t>ab%cd$</t>
-  </si>
-  <si>
-    <t>pwd098</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>password_mismatch:The two password fields didn’t match.</t>
-  </si>
-  <si>
-    <t>User2</t>
-  </si>
-  <si>
-    <t>ritu567</t>
-  </si>
-  <si>
-    <t>User3</t>
-  </si>
-  <si>
-    <t>"12345678"</t>
-  </si>
-  <si>
-    <t>User4</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>" "</t>
-  </si>
-  <si>
-    <t>User5</t>
-  </si>
-  <si>
-    <t>tets4455</t>
-  </si>
-  <si>
-    <t>User6</t>
-  </si>
-  <si>
-    <t>password66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MyNameIsIncorrectPassword.DoNotTryMeToCorrect.ToTtestMyTestCaseForMyDS-AlgoProjectAAndHereIamTestingForNegativeScenarioToTestUserNameExceed150Characters. </t>
-  </si>
-  <si>
-    <t>kkk098</t>
-  </si>
-  <si>
-    <t>User7</t>
-  </si>
-  <si>
-    <t>Test1177</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>sonali</t>
-  </si>
-  <si>
-    <t>Dsalgo@1</t>
+    <t>User</t>
+  </si>
+  <si>
+    <t>UserInvalid</t>
+  </si>
+  <si>
+    <t>Passwordinvalid</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>sdetorganizers@gmail.com</t>
+  </si>
+  <si>
+    <t>UIHackathon@02</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>UITest</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Java tutorial</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>NoOfClasses</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>UItesters11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color indexed="17"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -145,38 +126,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1334,194 +1297,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AECB39-022E-C440-A2DD-E283837CEA26}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="60.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="104.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E46D8369-9E31-C943-81A0-1901F85A9254}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9F67AA4D-3A24-B345-8E19-908F365E8E21}"/>
+    <hyperlink ref="B6" r:id="rId3" display="mailto:UIHackathon@02" xr:uid="{08A2F433-8CA0-1C40-8260-B315A9815A32}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -1533,7 +1446,7 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1547,7 +1460,7 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1555,14 +1468,66 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A5BB4C-78E8-4235-BB08-BDD5F2542772}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sdetorganizers@gmail.com" xr:uid="{BA871B86-C228-47C5-8445-C5AF53AE1AE5}"/>
+    <hyperlink ref="B2" r:id="rId2" display="UIHackathon@02" xr:uid="{84521D8D-E0E9-4ED6-913F-3C2BDFE37A2A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1571,11 +1536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8389F19E-6C3C-43CB-A26D-C0205F142CEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>